<commit_message>
standard template added digital asset tab fix
</commit_message>
<xml_diff>
--- a/data/templates/standard_template.xlsx
+++ b/data/templates/standard_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdangi\Downloads\ETL Pipeline Project - Phase 1\Vendor Portal Setup\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdangi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91DD38F-57BC-4E36-8CF2-167105BC1219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A903A048-1513-43BA-8BCF-EED3469897FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3225" yWindow="2145" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_Master" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="Part_Interchange" sheetId="5" r:id="rId5"/>
     <sheet name="Packages" sheetId="6" r:id="rId6"/>
     <sheet name="Digital_Assets" sheetId="7" state="hidden" r:id="rId7"/>
-    <sheet name="Pricing" sheetId="8" r:id="rId8"/>
-    <sheet name="EHC" sheetId="9" r:id="rId9"/>
-    <sheet name="CountryCodes" sheetId="10" state="hidden" r:id="rId10"/>
+    <sheet name="Digital Assets" sheetId="11" r:id="rId8"/>
+    <sheet name="Pricing" sheetId="8" r:id="rId9"/>
+    <sheet name="EHC" sheetId="9" r:id="rId10"/>
+    <sheet name="CountryCodes" sheetId="10" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
   <si>
     <t>Part Number</t>
   </si>
@@ -263,9 +264,6 @@
     <t>Order of Occurrence</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
     <t>Extended Info Type</t>
   </si>
   <si>
@@ -290,16 +288,10 @@
     <t>Net Cost</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>121212121212</t>
-  </si>
-  <si>
-    <t>UPC</t>
+    <t>FilePath</t>
+  </si>
+  <si>
+    <t>Asset Change Type</t>
   </si>
 </sst>
 </file>
@@ -812,10 +804,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,32 +849,6 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -937,6 +903,85 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA19AB5-6FE3-4135-9DAC-A88E20833ABE}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FFFCBF-33ED-4AA6-BD9C-C79EA941CCDD}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B244"/>
@@ -953,16 +998,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3381,11 +3426,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3411,11 +3454,6 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3464,7 +3502,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -3572,10 +3610,10 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3747,7 +3785,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -3770,12 +3808,59 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32639606-26D3-4D32-BD95-E9638552A4E2}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{BEB7556E-817A-4D6C-86CC-9A00C7E40638}">
+      <formula1>"Primary, Additional, LinArt, PDFs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{3B92E3ED-26FB-48D2-BCD5-B2550E4D354E}">
+      <formula1>"Add, Modify, Delete"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,7 +3918,7 @@
         <v>45</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>46</v>
@@ -3905,83 +3990,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA19AB5-6FE3-4135-9DAC-A88E20833ABE}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>